<commit_message>
fixed schedule, added fol notes
</commit_message>
<xml_diff>
--- a/schedule-2020.xlsx
+++ b/schedule-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skalakm\google\teaching\ai\githubrepo\dickinsonaifall2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B621E1-C0E0-41AC-993C-E6CA3B5C4886}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C7F4ED-8DA9-4539-92E3-C16FE9BD086A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25125" yWindow="2535" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26400" yWindow="2115" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -900,8 +900,8 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1011,7 +1011,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="20">
-        <f t="shared" ref="C5:C29" si="0">C3+7</f>
+        <f t="shared" ref="C5:C16" si="0">C3+7</f>
         <v>44070</v>
       </c>
       <c r="D5" s="32"/>
@@ -1241,8 +1241,8 @@
         <v>62</v>
       </c>
       <c r="C16" s="20">
-        <f t="shared" si="0"/>
-        <v>44110</v>
+        <f>C15+7</f>
+        <v>44112</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>32</v>
@@ -1263,8 +1263,8 @@
         <v>65</v>
       </c>
       <c r="C17" s="20">
-        <f t="shared" si="0"/>
-        <v>44112</v>
+        <f>C16+2</f>
+        <v>44114</v>
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="18" t="s">
@@ -1283,8 +1283,8 @@
         <v>62</v>
       </c>
       <c r="C18" s="20">
-        <f t="shared" si="0"/>
-        <v>44117</v>
+        <f>C16+7</f>
+        <v>44119</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="25" t="s">
@@ -1304,8 +1304,8 @@
         <v>65</v>
       </c>
       <c r="C19" s="20">
-        <f t="shared" si="0"/>
-        <v>44119</v>
+        <f>C17+7</f>
+        <v>44121</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="25" t="s">
@@ -1324,8 +1324,8 @@
         <v>62</v>
       </c>
       <c r="C20" s="20">
-        <f t="shared" si="0"/>
-        <v>44124</v>
+        <f>C18+7</f>
+        <v>44126</v>
       </c>
       <c r="D20" s="45" t="s">
         <v>44</v>
@@ -1342,8 +1342,8 @@
         <v>65</v>
       </c>
       <c r="C21" s="20">
-        <f t="shared" si="0"/>
-        <v>44126</v>
+        <f>C19+7</f>
+        <v>44128</v>
       </c>
       <c r="D21" s="32" t="s">
         <v>53</v>
@@ -1362,8 +1362,8 @@
         <v>62</v>
       </c>
       <c r="C22" s="20">
-        <f t="shared" si="0"/>
-        <v>44131</v>
+        <f>C20+7</f>
+        <v>44133</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>5</v>
@@ -1380,8 +1380,8 @@
         <v>65</v>
       </c>
       <c r="C23" s="20">
-        <f t="shared" si="0"/>
-        <v>44133</v>
+        <f>C21+7</f>
+        <v>44135</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="25" t="s">
@@ -1397,11 +1397,11 @@
         <v>24</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="20">
-        <f t="shared" si="0"/>
-        <v>44138</v>
+        <f>C22+7</f>
+        <v>44140</v>
       </c>
       <c r="D24" s="42" t="s">
         <v>52</v>
@@ -1416,11 +1416,11 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C25" s="20">
-        <f t="shared" si="0"/>
-        <v>44140</v>
+        <f>C23+7</f>
+        <v>44142</v>
       </c>
       <c r="D25" s="43"/>
       <c r="E25" s="22" t="s">
@@ -1438,11 +1438,11 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C26" s="20">
-        <f t="shared" si="0"/>
-        <v>44145</v>
+        <f>C24+7</f>
+        <v>44147</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="39" t="s">
@@ -1458,11 +1458,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C27" s="20">
-        <f t="shared" si="0"/>
-        <v>44147</v>
+        <f>C25+7</f>
+        <v>44149</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="33" t="s">
@@ -1478,11 +1478,11 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C28" s="20">
-        <f t="shared" si="0"/>
-        <v>44152</v>
+        <f>C26+7</f>
+        <v>44154</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="18" t="s">
@@ -1498,11 +1498,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C29" s="20">
-        <f t="shared" si="0"/>
-        <v>44154</v>
+        <f>C27+7</f>
+        <v>44156</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="18" t="s">

</xml_diff>

<commit_message>
added neural net exercise
</commit_message>
<xml_diff>
--- a/schedule-2020.xlsx
+++ b/schedule-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skalakm\google\teaching\ai\githubrepo\dickinsonaifall2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C7F4ED-8DA9-4539-92E3-C16FE9BD086A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12530531-865A-44B0-AD98-C22226505E41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26400" yWindow="2115" windowWidth="19185" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>Class number</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>PA3</t>
-  </si>
-  <si>
-    <t>PA4</t>
   </si>
   <si>
     <t>FP1</t>
@@ -901,7 +898,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E26" sqref="E26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,16 +924,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H1" s="5"/>
     </row>
@@ -945,19 +942,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="20">
         <v>44061</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -966,20 +963,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="20">
         <f>C2+2</f>
         <v>44063</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -988,7 +985,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="20">
         <f>C2+7</f>
@@ -996,7 +993,7 @@
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="12">
         <v>3.5</v>
@@ -1008,15 +1005,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="20">
-        <f t="shared" ref="C5:C16" si="0">C3+7</f>
+        <f t="shared" ref="C5:C15" si="0">C3+7</f>
         <v>44070</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="12">
         <v>3.6</v>
@@ -1028,20 +1025,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="20">
         <f t="shared" si="0"/>
         <v>44075</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1050,7 +1047,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="20">
         <f t="shared" si="0"/>
@@ -1060,10 +1057,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1072,7 +1069,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="20">
         <f t="shared" si="0"/>
@@ -1080,7 +1077,7 @@
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="12">
         <v>5.3</v>
@@ -1094,7 +1091,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="20">
         <f t="shared" si="0"/>
@@ -1102,7 +1099,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="12">
         <v>5.4</v>
@@ -1114,7 +1111,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="20">
         <f t="shared" si="0"/>
@@ -1122,10 +1119,10 @@
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -1134,7 +1131,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="20">
         <f t="shared" si="0"/>
@@ -1142,7 +1139,7 @@
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
@@ -1152,20 +1149,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="20">
         <f t="shared" si="0"/>
         <v>44096</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="14"/>
     </row>
@@ -1174,20 +1171,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="20">
         <f t="shared" si="0"/>
         <v>44098</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>7</v>
@@ -1198,19 +1195,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="20">
         <f t="shared" si="0"/>
         <v>44103</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="38"/>
       <c r="G14" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1218,19 +1215,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="20">
         <f t="shared" si="0"/>
         <v>44105</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="35"/>
       <c r="G15" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1238,20 +1235,20 @@
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="20">
         <f>C15+7</f>
         <v>44112</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="14"/>
     </row>
@@ -1260,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="20">
         <f>C16+2</f>
@@ -1268,10 +1265,10 @@
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="14"/>
     </row>
@@ -1280,18 +1277,18 @@
         <v>17</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="20">
-        <f>C16+7</f>
+        <f t="shared" ref="C18:C29" si="1">C16+7</f>
         <v>44119</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="14"/>
       <c r="I18" s="23"/>
@@ -1301,18 +1298,18 @@
         <v>18</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="20">
-        <f>C17+7</f>
+        <f t="shared" si="1"/>
         <v>44121</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -1321,14 +1318,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="20">
-        <f>C18+7</f>
+        <f t="shared" si="1"/>
         <v>44126</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="45"/>
@@ -1339,14 +1336,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="20">
-        <f>C19+7</f>
+        <f t="shared" si="1"/>
         <v>44128</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
@@ -1359,10 +1356,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="20">
-        <f>C20+7</f>
+        <f t="shared" si="1"/>
         <v>44133</v>
       </c>
       <c r="D22" s="32" t="s">
@@ -1377,18 +1374,18 @@
         <v>22</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="20">
-        <f>C21+7</f>
+        <f t="shared" si="1"/>
         <v>44135</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="2"/>
     </row>
@@ -1397,40 +1394,40 @@
         <v>24</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="20">
-        <f>C22+7</f>
+        <f t="shared" si="1"/>
         <v>44140</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="20">
-        <f>C23+7</f>
+        <f t="shared" si="1"/>
         <v>44142</v>
       </c>
       <c r="D25" s="43"/>
       <c r="E25" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1438,39 +1435,37 @@
         <v>25</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="20">
-        <f>C24+7</f>
+        <f t="shared" si="1"/>
         <v>44147</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="41"/>
-      <c r="G26" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="20">
-        <f>C25+7</f>
+        <f t="shared" si="1"/>
         <v>44149</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="35"/>
       <c r="G27" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1478,18 +1473,18 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="20">
-        <f>C26+7</f>
+        <f t="shared" si="1"/>
         <v>44154</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -1498,19 +1493,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="20">
-        <f>C27+7</f>
+        <f t="shared" si="1"/>
         <v>44156</v>
       </c>
       <c r="D29" s="44"/>
       <c r="E29" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>